<commit_message>
its about search of cell value in all row of column
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11020"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hirenkumarpatel/Desktop/pyth/exelPytha/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="288" yWindow="96" windowWidth="9540" windowHeight="4512"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="10400" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Apples</t>
   </si>
@@ -34,12 +39,15 @@
   </si>
   <si>
     <t>Strawberries</t>
+  </si>
+  <si>
+    <t>wer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -86,6 +94,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,6 +104,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -143,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +188,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -211,6 +240,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -386,19 +432,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>42099.565300925926</v>
       </c>
@@ -409,7 +455,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>42099.153738425928</v>
       </c>
@@ -420,7 +466,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>42100.532534722224</v>
       </c>
@@ -431,7 +477,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>42102.374803240738</v>
       </c>
@@ -442,7 +488,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>42104.088194444441</v>
       </c>
@@ -453,7 +499,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>42104.757372685184</v>
       </c>
@@ -464,7 +510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>42104.111643518518</v>
       </c>
@@ -473,6 +519,14 @@
       </c>
       <c r="C7" s="3">
         <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="4">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -482,24 +536,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>